<commit_message>
ADDS handling for AbuseRates
</commit_message>
<xml_diff>
--- a/inst/extdata/src_dat/child outcomes data.xlsx
+++ b/inst/extdata/src_dat/child outcomes data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="10035"/>
+    <workbookView xWindow="480" yWindow="48" windowWidth="22992" windowHeight="10032"/>
   </bookViews>
   <sheets>
     <sheet name="Abuse data" sheetId="1" r:id="rId1"/>
@@ -1238,24 +1238,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
@@ -1332,7 +1334,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>12</v>
       </c>
@@ -1433,7 +1435,7 @@
         <v>9.8490122438172858E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A4+1</f>
         <v>13</v>
@@ -1535,7 +1537,7 @@
         <v>8.9029958841739892E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" ref="A6:A10" si="20">A5+1</f>
         <v>14</v>
@@ -1637,7 +1639,7 @@
         <v>8.3776069929760111E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="20"/>
         <v>15</v>
@@ -1739,7 +1741,7 @@
         <v>7.8784599462691673E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="20"/>
         <v>16</v>
@@ -1841,7 +1843,7 @@
         <v>7.4048032000090941E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="20"/>
         <v>17</v>
@@ -1943,7 +1945,7 @@
         <v>6.9558378543980864E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="20"/>
         <v>18</v>
@@ -1993,7 +1995,7 @@
         <v>0.10051940869907326</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" si="9"/>
+        <f>W67</f>
         <v>7.2758715777634986E-2</v>
       </c>
       <c r="N10" s="2">
@@ -2017,8 +2019,8 @@
         <v>0.15134453176577095</v>
       </c>
       <c r="S10" s="2">
-        <f>N10*$B$36</f>
-        <v>0</v>
+        <f>K67</f>
+        <v>0.11270541088783727</v>
       </c>
       <c r="T10" s="2">
         <f t="shared" si="24"/>
@@ -2045,7 +2047,7 @@
         <v>6.5307279512189356E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -2071,12 +2073,12 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>25</v>
       </c>
@@ -2110,7 +2112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29"/>
       <c r="B20" s="30"/>
       <c r="C20" s="33" t="s">
@@ -2166,7 +2168,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="31"/>
       <c r="B21" s="32"/>
       <c r="C21" s="34"/>
@@ -2190,7 +2192,7 @@
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
     </row>
-    <row r="22" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>39</v>
       </c>
@@ -2252,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="27"/>
       <c r="B23" s="8" t="s">
         <v>41</v>
@@ -2312,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="27"/>
       <c r="B24" s="8" t="s">
         <v>42</v>
@@ -2381,7 +2383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="27"/>
       <c r="B25" s="8" t="s">
         <v>43</v>
@@ -2441,7 +2443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="27"/>
       <c r="B26" s="8" t="s">
         <v>44</v>
@@ -2501,7 +2503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="28"/>
       <c r="B27" s="9" t="s">
         <v>45</v>
@@ -2561,7 +2563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="H28" s="3"/>
       <c r="J28">
         <f>J22*$C22+J23*$C23+J24*$C24+J25*$C25+J26*$C26+J27*$C27</f>
@@ -2612,7 +2614,7 @@
         <v>-1.9309999999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="J29">
         <f>EXP(-J28)</f>
         <v>4.4149654127785762</v>
@@ -2662,7 +2664,7 @@
         <v>6.8964031977265314</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>95</v>
       </c>
@@ -2723,7 +2725,7 @@
         <v>0.12663993655844624</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="I31" t="s">
         <v>47</v>
       </c>
@@ -2765,7 +2767,7 @@
       <c r="Z31" s="1"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="O32" s="1"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
@@ -2780,7 +2782,7 @@
       <c r="Z32" s="1"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="11"/>
       <c r="I33" t="s">
@@ -2805,7 +2807,7 @@
       <c r="AE33" s="1"/>
       <c r="AF33" s="1"/>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="J34" t="s">
         <v>80</v>
@@ -2820,7 +2822,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="J35" t="s">
         <v>48</v>
@@ -2847,7 +2849,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="I36">
         <v>11</v>
@@ -2878,7 +2880,7 @@
         <v>0.18182969567174331</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I37">
         <f>I36+1</f>
         <v>12</v>
@@ -2929,7 +2931,7 @@
         <v>9.8772891706703572E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>94</v>
       </c>
@@ -2986,7 +2988,7 @@
         <v>9.3048386115668652E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>51</v>
       </c>
@@ -3043,7 +3045,7 @@
         <v>8.7597868656478298E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -3100,7 +3102,7 @@
         <v>8.2414909883604531E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I41">
         <f t="shared" si="34"/>
         <v>16</v>
@@ -3151,7 +3153,7 @@
         <v>7.7492410914695414E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I42">
         <f t="shared" si="34"/>
         <v>17</v>
@@ -3202,7 +3204,7 @@
         <v>7.2822719051762075E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I43">
         <f t="shared" si="34"/>
         <v>18</v>
@@ -3253,7 +3255,7 @@
         <v>6.8397736362632119E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I45" t="s">
         <v>92</v>
       </c>
@@ -3262,7 +3264,7 @@
       </c>
       <c r="O45" s="1"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="J46" t="s">
         <v>84</v>
       </c>
@@ -3276,7 +3278,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="J47" t="s">
         <v>48</v>
       </c>
@@ -3302,7 +3304,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I48">
         <v>11</v>
       </c>
@@ -3332,7 +3334,7 @@
         <v>0.18182969567174331</v>
       </c>
     </row>
-    <row r="49" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I49">
         <f>I48+1</f>
         <v>12</v>
@@ -3383,7 +3385,7 @@
         <v>0.17179850438210215</v>
       </c>
     </row>
-    <row r="50" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I50">
         <f t="shared" ref="I50:I55" si="45">I49+1</f>
         <v>13</v>
@@ -3434,7 +3436,7 @@
         <v>0.13384100564837365</v>
       </c>
     </row>
-    <row r="51" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I51">
         <f t="shared" si="45"/>
         <v>14</v>
@@ -3485,7 +3487,7 @@
         <v>0.12659598860439431</v>
       </c>
     </row>
-    <row r="52" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I52">
         <f t="shared" si="45"/>
         <v>15</v>
@@ -3536,7 +3538,7 @@
         <v>0.11964275618982616</v>
       </c>
     </row>
-    <row r="53" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I53">
         <f t="shared" si="45"/>
         <v>16</v>
@@ -3587,7 +3589,7 @@
         <v>0.11298053268892955</v>
       </c>
     </row>
-    <row r="54" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I54">
         <f t="shared" si="45"/>
         <v>17</v>
@@ -3638,7 +3640,7 @@
         <v>0.10660719638400723</v>
       </c>
     </row>
-    <row r="55" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I55">
         <f t="shared" si="45"/>
         <v>18</v>
@@ -3689,7 +3691,7 @@
         <v>0.10051940869907326</v>
       </c>
     </row>
-    <row r="57" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I57" t="s">
         <v>93</v>
       </c>
@@ -3697,7 +3699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="8:23" x14ac:dyDescent="0.3">
       <c r="J58" t="s">
         <v>88</v>
       </c>
@@ -3711,7 +3713,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="59" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="8:23" x14ac:dyDescent="0.3">
       <c r="J59" t="s">
         <v>48</v>
       </c>
@@ -3737,7 +3739,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I60">
         <v>11</v>
       </c>
@@ -3767,7 +3769,7 @@
         <v>0.18182969567174331</v>
       </c>
     </row>
-    <row r="61" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="8:23" x14ac:dyDescent="0.3">
       <c r="H61" s="1"/>
       <c r="I61">
         <f>I60+1</f>
@@ -3819,7 +3821,7 @@
         <v>0.10894909707638729</v>
       </c>
     </row>
-    <row r="62" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I62">
         <f t="shared" ref="I62:I67" si="57">I61+1</f>
         <v>13</v>
@@ -3870,7 +3872,7 @@
         <v>9.8690335626198764E-2</v>
       </c>
     </row>
-    <row r="63" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I63">
         <f t="shared" si="57"/>
         <v>14</v>
@@ -3921,7 +3923,7 @@
         <v>9.2969730172366247E-2</v>
       </c>
     </row>
-    <row r="64" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="8:23" x14ac:dyDescent="0.3">
       <c r="I64">
         <f t="shared" si="57"/>
         <v>15</v>
@@ -3972,7 +3974,7 @@
         <v>8.7523027495796449E-2</v>
       </c>
     </row>
-    <row r="65" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I65">
         <f t="shared" si="57"/>
         <v>16</v>
@@ -4023,7 +4025,7 @@
         <v>8.2343787890275549E-2</v>
       </c>
     </row>
-    <row r="66" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I66">
         <f t="shared" si="57"/>
         <v>17</v>
@@ -4074,7 +4076,7 @@
         <v>7.7424903885994656E-2</v>
       </c>
     </row>
-    <row r="67" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I67">
         <f t="shared" si="57"/>
         <v>18</v>
@@ -4148,28 +4150,28 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -4246,7 +4248,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12</v>
       </c>
@@ -4347,7 +4349,7 @@
         <v>6.0138786840652658E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>13</v>
@@ -4449,7 +4451,7 @@
         <v>6.9647157565001047E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:A11" si="24">A6+1</f>
         <v>14</v>
@@ -4551,7 +4553,7 @@
         <v>8.0443889665049603E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="24"/>
         <v>15</v>
@@ -4653,7 +4655,7 @@
         <v>9.266408977527113E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="24"/>
         <v>16</v>
@@ -4755,7 +4757,7 @@
         <v>0.1064450605052412</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="24"/>
         <v>17</v>
@@ -4857,7 +4859,7 @@
         <v>0.12192234785265216</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="24"/>
         <v>18</v>
@@ -4959,7 +4961,7 @@
         <v>0.13922465565303327</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -4985,7 +4987,7 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -5014,7 +5016,7 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>A4</f>
         <v>Age</v>
@@ -5116,7 +5118,7 @@
         <v>m.h.X5</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" ref="A15:A20" si="26">A5</f>
         <v>12</v>
@@ -5218,7 +5220,7 @@
         <v>0.14995774555657526</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="26"/>
         <v>13</v>
@@ -5320,7 +5322,7 @@
         <v>0.17035204037908908</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="26"/>
         <v>14</v>
@@ -5422,7 +5424,7 @@
         <v>0.1928241918647402</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="26"/>
         <v>15</v>
@@ -5524,7 +5526,7 @@
         <v>0.2174205760205149</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="26"/>
         <v>16</v>
@@ -5626,7 +5628,7 @@
         <v>0.2441453798977363</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="26"/>
         <v>17</v>
@@ -5728,7 +5730,7 @@
         <v>0.27295251423225325</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <f>A11</f>
         <v>18</v>
@@ -5830,12 +5832,12 @@
         <v>0.30373896298734987</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="J28" t="s">
         <v>25</v>
       </c>
@@ -5846,7 +5848,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -5869,7 +5871,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39"/>
       <c r="B31" s="40"/>
       <c r="C31" s="43" t="s">
@@ -5925,7 +5927,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:25" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="41"/>
       <c r="B32" s="42"/>
       <c r="C32" s="44"/>
@@ -5949,7 +5951,7 @@
       <c r="V32" s="4"/>
       <c r="W32" s="4"/>
     </row>
-    <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="37" t="s">
         <v>57</v>
       </c>
@@ -6011,7 +6013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A34" s="38"/>
       <c r="B34" s="12" t="s">
         <v>41</v>
@@ -6071,7 +6073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
       <c r="B35" s="12" t="s">
         <v>42</v>
@@ -6140,7 +6142,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A36" s="38"/>
       <c r="B36" s="12" t="s">
         <v>43</v>
@@ -6200,7 +6202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A37" s="38"/>
       <c r="B37" s="12" t="s">
         <v>44</v>
@@ -6260,7 +6262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:32" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:32" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A38" s="38"/>
       <c r="B38" s="12" t="s">
         <v>56</v>
@@ -6320,7 +6322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18"/>
       <c r="B39" s="19" t="s">
         <v>45</v>
@@ -6380,7 +6382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.3">
       <c r="H40" s="3"/>
       <c r="J40">
         <f>J33*$C33+J34*$C34+J35*$C35+J36*$C36+J37*$C37+J38*$C38+J39*$C39</f>
@@ -6431,7 +6433,7 @@
         <v>-1.3490000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.3">
       <c r="J41">
         <f>EXP(-J40)</f>
         <v>3.8037978429971542</v>
@@ -6481,7 +6483,7 @@
         <v>3.8535700332362999</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -6542,7 +6544,7 @@
         <v>0.20603390764987323</v>
       </c>
     </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.3">
       <c r="I43" t="s">
         <v>47</v>
       </c>
@@ -6584,7 +6586,7 @@
       <c r="Z43" s="1"/>
       <c r="AA43" s="1"/>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>94</v>
       </c>
@@ -6605,7 +6607,7 @@
       <c r="Z44" s="1"/>
       <c r="AA44" s="1"/>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>51</v>
       </c>
@@ -6641,7 +6643,7 @@
       <c r="AE45" s="1"/>
       <c r="AF45" s="1"/>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>52</v>
       </c>
@@ -6661,7 +6663,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="J47" t="s">
         <v>48</v>
@@ -6688,7 +6690,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="I48">
         <v>11</v>
@@ -6719,7 +6721,7 @@
         <v>5.6786180808788486E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="I49">
         <f>I48+1</f>
@@ -6771,7 +6773,7 @@
         <v>5.9635640495214338E-2</v>
       </c>
     </row>
-    <row r="50" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I50">
         <f t="shared" ref="I50:I55" si="63">I49+1</f>
         <v>13</v>
@@ -6822,7 +6824,7 @@
         <v>6.8489779559944258E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I51">
         <f t="shared" si="63"/>
         <v>14</v>
@@ -6873,7 +6875,7 @@
         <v>7.8535874423254479E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I52">
         <f t="shared" si="63"/>
         <v>15</v>
@@ -6924,7 +6926,7 @@
         <v>8.9896510804592988E-2</v>
       </c>
     </row>
-    <row r="53" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I53">
         <f t="shared" si="63"/>
         <v>16</v>
@@ -6975,7 +6977,7 @@
         <v>0.10269543582069027</v>
       </c>
     </row>
-    <row r="54" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I54">
         <f t="shared" si="63"/>
         <v>17</v>
@@ -7026,7 +7028,7 @@
         <v>0.11705373594432186</v>
       </c>
     </row>
-    <row r="55" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I55">
         <f t="shared" si="63"/>
         <v>18</v>
@@ -7077,7 +7079,7 @@
         <v>0.1330849768166428</v>
       </c>
     </row>
-    <row r="57" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I57" t="s">
         <v>97</v>
       </c>
@@ -7089,7 +7091,7 @@
       </c>
       <c r="O57" s="1"/>
     </row>
-    <row r="58" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:23" x14ac:dyDescent="0.3">
       <c r="J58" t="s">
         <v>99</v>
       </c>
@@ -7103,7 +7105,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:23" x14ac:dyDescent="0.3">
       <c r="J59" t="s">
         <v>48</v>
       </c>
@@ -7129,7 +7131,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I60">
         <v>11</v>
       </c>
@@ -7159,7 +7161,7 @@
         <v>5.6786180808788486E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I61">
         <f>I60+1</f>
         <v>12</v>
@@ -7210,7 +7212,7 @@
         <v>8.2586842606058614E-2</v>
       </c>
     </row>
-    <row r="62" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I62">
         <f t="shared" ref="I62:I67" si="71">I61+1</f>
         <v>13</v>
@@ -7261,7 +7263,7 @@
         <v>9.2188211326529282E-2</v>
       </c>
     </row>
-    <row r="63" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I63">
         <f t="shared" si="71"/>
         <v>14</v>
@@ -7312,7 +7314,7 @@
         <v>0.1052710883891488</v>
       </c>
     </row>
-    <row r="64" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:23" x14ac:dyDescent="0.3">
       <c r="I64">
         <f t="shared" si="71"/>
         <v>15</v>
@@ -7363,7 +7365,7 @@
         <v>0.11993541997209507</v>
       </c>
     </row>
-    <row r="65" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I65">
         <f t="shared" si="71"/>
         <v>16</v>
@@ -7414,7 +7416,7 @@
         <v>0.13629273002326803</v>
       </c>
     </row>
-    <row r="66" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I66">
         <f t="shared" si="71"/>
         <v>17</v>
@@ -7465,7 +7467,7 @@
         <v>0.15443989716784226</v>
       </c>
     </row>
-    <row r="67" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I67">
         <f t="shared" si="71"/>
         <v>18</v>
@@ -7516,7 +7518,7 @@
         <v>0.17445215090419683</v>
       </c>
     </row>
-    <row r="69" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I69" t="s">
         <v>107</v>
       </c>
@@ -7527,7 +7529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J70" t="s">
         <v>108</v>
       </c>
@@ -7541,7 +7543,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="71" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J71" t="s">
         <v>48</v>
       </c>
@@ -7567,7 +7569,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I72">
         <v>11</v>
       </c>
@@ -7597,7 +7599,7 @@
         <v>5.6786180808788486E-2</v>
       </c>
     </row>
-    <row r="73" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I73">
         <f>I72+1</f>
         <v>12</v>
@@ -7648,7 +7650,7 @@
         <v>9.027636511993109E-2</v>
       </c>
     </row>
-    <row r="74" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I74">
         <f t="shared" ref="I74:I79" si="83">I73+1</f>
         <v>13</v>
@@ -7699,7 +7701,7 @@
         <v>0.10008586033603298</v>
       </c>
     </row>
-    <row r="75" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I75">
         <f t="shared" si="83"/>
         <v>14</v>
@@ -7750,7 +7752,7 @@
         <v>0.11413144566820385</v>
       </c>
     </row>
-    <row r="76" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I76">
         <f t="shared" si="83"/>
         <v>15</v>
@@ -7801,7 +7803,7 @@
         <v>0.12982872201365486</v>
       </c>
     </row>
-    <row r="77" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I77">
         <f t="shared" si="83"/>
         <v>16</v>
@@ -7852,7 +7854,7 @@
         <v>0.14728095246135559</v>
       </c>
     </row>
-    <row r="78" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I78">
         <f t="shared" si="83"/>
         <v>17</v>
@@ -7903,7 +7905,7 @@
         <v>0.16657252414397133</v>
       </c>
     </row>
-    <row r="79" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I79">
         <f t="shared" si="83"/>
         <v>18</v>
@@ -7954,7 +7956,7 @@
         <v>0.1877615070306955</v>
       </c>
     </row>
-    <row r="81" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I81" t="s">
         <v>112</v>
       </c>
@@ -7965,7 +7967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J82" t="s">
         <v>113</v>
       </c>
@@ -7979,7 +7981,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="83" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J83" t="s">
         <v>48</v>
       </c>
@@ -8005,7 +8007,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="84" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I84">
         <v>11</v>
       </c>
@@ -8035,7 +8037,7 @@
         <v>5.6786180808788486E-2</v>
       </c>
     </row>
-    <row r="85" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I85">
         <f>I84+1</f>
         <v>12</v>
@@ -8086,7 +8088,7 @@
         <v>0.15115219942802108</v>
       </c>
     </row>
-    <row r="86" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I86">
         <f t="shared" ref="I86:I91" si="95">I85+1</f>
         <v>13</v>
@@ -8137,7 +8139,7 @@
         <v>0.16187209217418533</v>
       </c>
     </row>
-    <row r="87" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I87">
         <f t="shared" si="95"/>
         <v>14</v>
@@ -8188,7 +8190,7 @@
         <v>0.1826118330759173</v>
       </c>
     </row>
-    <row r="88" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I88">
         <f t="shared" si="95"/>
         <v>15</v>
@@ -8239,7 +8241,7 @@
         <v>0.20527077203822922</v>
       </c>
     </row>
-    <row r="89" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I89">
         <f t="shared" si="95"/>
         <v>16</v>
@@ -8290,7 +8292,7 @@
         <v>0.22984150185422531</v>
       </c>
     </row>
-    <row r="90" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I90">
         <f t="shared" si="95"/>
         <v>17</v>
@@ -8341,7 +8343,7 @@
         <v>0.25626950146858768</v>
       </c>
     </row>
-    <row r="91" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I91">
         <f t="shared" si="95"/>
         <v>18</v>
@@ -8392,7 +8394,7 @@
         <v>0.28444759676866466</v>
       </c>
     </row>
-    <row r="93" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I93" t="s">
         <v>117</v>
       </c>
@@ -8403,7 +8405,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J94" t="s">
         <v>118</v>
       </c>
@@ -8417,7 +8419,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="95" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J95" t="s">
         <v>48</v>
       </c>
@@ -8443,7 +8445,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="96" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I96">
         <v>11</v>
       </c>
@@ -8473,7 +8475,7 @@
         <v>5.6786180808788486E-2</v>
       </c>
     </row>
-    <row r="97" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I97">
         <f>I96+1</f>
         <v>12</v>
@@ -8524,7 +8526,7 @@
         <v>0.19921255814933539</v>
       </c>
     </row>
-    <row r="98" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I98">
         <f t="shared" ref="I98:I103" si="107">I97+1</f>
         <v>13</v>
@@ -8575,7 +8577,7 @@
         <v>0.20974317915193691</v>
       </c>
     </row>
-    <row r="99" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I99">
         <f t="shared" si="107"/>
         <v>14</v>
@@ -8626,7 +8628,7 @@
         <v>0.23466861309473777</v>
       </c>
     </row>
-    <row r="100" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I100">
         <f t="shared" si="107"/>
         <v>15</v>
@@ -8677,7 +8679,7 @@
         <v>0.26143532747980991</v>
       </c>
     </row>
-    <row r="101" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I101">
         <f t="shared" si="107"/>
         <v>16</v>
@@ -8728,7 +8730,7 @@
         <v>0.28992581503527098</v>
       </c>
     </row>
-    <row r="102" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I102">
         <f t="shared" si="107"/>
         <v>17</v>
@@ -8779,7 +8781,7 @@
         <v>0.3199664915404814</v>
       </c>
     </row>
-    <row r="103" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I103">
         <f t="shared" si="107"/>
         <v>18</v>
@@ -8830,7 +8832,7 @@
         <v>0.35132836382678551</v>
       </c>
     </row>
-    <row r="105" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I105" t="s">
         <v>122</v>
       </c>
@@ -8841,7 +8843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J106" t="s">
         <v>123</v>
       </c>
@@ -8855,7 +8857,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="107" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="9:23" x14ac:dyDescent="0.3">
       <c r="J107" t="s">
         <v>48</v>
       </c>
@@ -8881,7 +8883,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="108" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I108">
         <v>11</v>
       </c>
@@ -8911,7 +8913,7 @@
         <v>5.6786180808788486E-2</v>
       </c>
     </row>
-    <row r="109" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I109">
         <f>I108+1</f>
         <v>12</v>
@@ -8962,7 +8964,7 @@
         <v>0.21460746499850836</v>
       </c>
     </row>
-    <row r="110" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I110">
         <f t="shared" ref="I110:I115" si="119">I109+1</f>
         <v>13</v>
@@ -9013,7 +9015,7 @@
         <v>0.22491130127072356</v>
       </c>
     </row>
-    <row r="111" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I111">
         <f t="shared" si="119"/>
         <v>14</v>
@@ -9064,7 +9066,7 @@
         <v>0.25098451361873508</v>
       </c>
     </row>
-    <row r="112" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I112">
         <f t="shared" si="119"/>
         <v>15</v>
@@ -9115,7 +9117,7 @@
         <v>0.2788329969838958</v>
       </c>
     </row>
-    <row r="113" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="113" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I113">
         <f t="shared" si="119"/>
         <v>16</v>
@@ -9166,7 +9168,7 @@
         <v>0.30830473406242848</v>
       </c>
     </row>
-    <row r="114" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="114" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I114">
         <f t="shared" si="119"/>
         <v>17</v>
@@ -9217,7 +9219,7 @@
         <v>0.3391916149673575</v>
       </c>
     </row>
-    <row r="115" spans="9:23" x14ac:dyDescent="0.25">
+    <row r="115" spans="9:23" x14ac:dyDescent="0.3">
       <c r="I115">
         <f t="shared" si="119"/>
         <v>18</v>
@@ -9289,22 +9291,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -9378,7 +9380,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
@@ -9479,7 +9481,7 @@
         <v>9.2088203872148888E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <f>A5+1</f>
         <v>7</v>
@@ -9581,7 +9583,7 @@
         <v>4.6044101936074444E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" ref="A7:A16" si="20">A6+1</f>
         <v>8</v>
@@ -9683,7 +9685,7 @@
         <v>4.6044101936074444E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="20"/>
         <v>9</v>
@@ -9785,7 +9787,7 @@
         <v>4.6044101936074444E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="20"/>
         <v>10</v>
@@ -9887,7 +9889,7 @@
         <v>4.6044101936074444E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="20"/>
         <v>11</v>
@@ -9989,7 +9991,7 @@
         <v>4.6044101936074444E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="20"/>
         <v>12</v>
@@ -10091,7 +10093,7 @@
         <v>4.6044101936074444E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="20"/>
         <v>13</v>
@@ -10193,7 +10195,7 @@
         <v>3.6835281548859559E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="20"/>
         <v>14</v>
@@ -10295,7 +10297,7 @@
         <v>3.6835281548859559E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="20"/>
         <v>15</v>
@@ -10397,7 +10399,7 @@
         <v>3.6835281548859559E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="20"/>
         <v>16</v>
@@ -10499,7 +10501,7 @@
         <v>5.5252922323289329E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="20"/>
         <v>17</v>
@@ -10601,32 +10603,32 @@
         <v>5.5252922323289329E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -10634,7 +10636,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -10642,7 +10644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -10650,7 +10652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -10658,7 +10660,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>70</v>
       </c>
@@ -10667,7 +10669,7 @@
         <v>7.6292470586644678E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>71</v>
       </c>
@@ -10675,7 +10677,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>72</v>
       </c>
@@ -10683,23 +10685,23 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B32" s="1"/>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>73</v>
       </c>
       <c r="B33" s="1"/>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>A24</f>
         <v>Dropout out rate constant, except grade one where it is double</v>
       </c>
       <c r="B34" s="1"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -10707,7 +10709,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -10715,7 +10717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>68</v>
       </c>
@@ -10723,7 +10725,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -10731,7 +10733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -10740,7 +10742,7 @@
         <v>2.3022050968037222E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>71</v>
       </c>
@@ -10748,7 +10750,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -10756,7 +10758,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -10764,7 +10766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>75</v>
       </c>
@@ -10772,7 +10774,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>76</v>
       </c>
@@ -10780,7 +10782,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>77</v>
       </c>
@@ -10788,7 +10790,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>78</v>
       </c>
@@ -10796,7 +10798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -10815,34 +10817,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="25" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="25" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -10919,7 +10921,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>13</v>
       </c>
@@ -11020,7 +11022,7 @@
         <v>0.10229322865649333</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>14</v>
       </c>
@@ -11121,7 +11123,7 @@
         <v>3.2409823295534837E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>15</v>
       </c>
@@ -11222,12 +11224,12 @@
         <v>4.0672266081934388E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -11304,7 +11306,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>13</v>
       </c>
@@ -11405,7 +11407,7 @@
         <v>0.15407385387469932</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>14</v>
       </c>
@@ -11506,7 +11508,7 @@
         <v>4.5174306657326468E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>15</v>
       </c>
@@ -11607,17 +11609,17 @@
         <v>5.444714348891147E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -11694,7 +11696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>13</v>
       </c>
@@ -11771,7 +11773,7 @@
         <v>0.10229322865649333</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>14</v>
       </c>
@@ -11848,7 +11850,7 @@
         <v>0.13470305195202817</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>15</v>
       </c>
@@ -11949,7 +11951,7 @@
         <v>0.17537531803396256</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -11975,7 +11977,7 @@
       <c r="X23" s="2"/>
       <c r="Y23" s="2"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
@@ -12001,7 +12003,7 @@
       <c r="X24" s="2"/>
       <c r="Y24" s="2"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>96</v>
       </c>
@@ -12030,7 +12032,7 @@
       <c r="X25" s="2"/>
       <c r="Y25" s="2"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f t="shared" ref="A26:Y26" si="6">A19</f>
         <v>Age</v>
@@ -12132,7 +12134,7 @@
         <v>m.h.X5</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>13</v>
       </c>
@@ -12209,7 +12211,7 @@
         <v>0.15407385387469932</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>14</v>
       </c>
@@ -12286,7 +12288,7 @@
         <v>0.19924816053202579</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>A22</f>
         <v>15</v>
@@ -12388,7 +12390,7 @@
         <v>0.25369530402093726</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -12414,7 +12416,7 @@
       <c r="X30" s="2"/>
       <c r="Y30" s="2"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -12440,12 +12442,12 @@
       <c r="X31" s="2"/>
       <c r="Y31" s="2"/>
     </row>
-    <row r="33" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J37" t="s">
         <v>25</v>
       </c>
@@ -12465,7 +12467,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J38" t="s">
         <v>128</v>
       </c>
@@ -12485,7 +12487,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>28</v>
       </c>
@@ -12526,7 +12528,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:39" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="39"/>
       <c r="B40" s="40"/>
       <c r="C40" s="43" t="s">
@@ -12618,7 +12620,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="41"/>
       <c r="B41" s="42"/>
       <c r="C41" s="44"/>
@@ -12656,7 +12658,7 @@
       <c r="AL41" s="4"/>
       <c r="AM41" s="4"/>
     </row>
-    <row r="42" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="37" t="s">
         <v>57</v>
       </c>
@@ -12756,7 +12758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A43" s="38"/>
       <c r="B43" s="12" t="s">
         <v>41</v>
@@ -12854,7 +12856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A44" s="38"/>
       <c r="B44" s="12" t="s">
         <v>42</v>
@@ -12975,7 +12977,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A45" s="38"/>
       <c r="B45" s="12" t="s">
         <v>43</v>
@@ -13073,7 +13075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A46" s="38"/>
       <c r="B46" s="12" t="s">
         <v>44</v>
@@ -13171,7 +13173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:39" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:39" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A47" s="38"/>
       <c r="B47" s="12" t="s">
         <v>56</v>
@@ -13269,7 +13271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:39" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="18"/>
       <c r="B48" s="19" t="s">
         <v>45</v>
@@ -13367,7 +13369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:39" x14ac:dyDescent="0.3">
       <c r="H49" s="3"/>
       <c r="J49">
         <f>J42*$C42+J43*$C43+J44*$C44+J45*$C45+J46*$C46+J47*$C47+J48*$C48</f>
@@ -13466,7 +13468,7 @@
         <v>-2.1050000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J50">
         <f>EXP(-J49)</f>
         <v>5.4412020416630202</v>
@@ -13564,7 +13566,7 @@
         <v>8.2071030095958122</v>
       </c>
     </row>
-    <row r="51" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -13678,7 +13680,7 @@
         <v>0.10861179667022099</v>
       </c>
     </row>
-    <row r="52" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:39" x14ac:dyDescent="0.3">
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
       <c r="Q52" s="1"/>
@@ -13699,7 +13701,7 @@
       <c r="AL52" s="1"/>
       <c r="AM52" s="1"/>
     </row>
-    <row r="53" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -13720,7 +13722,7 @@
       <c r="Z53" s="1"/>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -13747,7 +13749,7 @@
       <c r="AE54" s="1"/>
       <c r="AF54" s="1"/>
     </row>
-    <row r="55" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -13755,17 +13757,17 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="56" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
     </row>
-    <row r="57" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
       <c r="J57" s="1"/>
       <c r="N57" s="1"/>
       <c r="R57" s="1"/>
       <c r="V57" s="1"/>
     </row>
-    <row r="58" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:39" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -13777,7 +13779,7 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="59" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="N59" s="1"/>
@@ -13788,7 +13790,7 @@
       <c r="V59" s="1"/>
       <c r="W59" s="1"/>
     </row>
-    <row r="60" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="N60" s="1"/>
@@ -13799,7 +13801,7 @@
       <c r="V60" s="1"/>
       <c r="W60" s="1"/>
     </row>
-    <row r="61" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="N61" s="1"/>
@@ -13810,7 +13812,7 @@
       <c r="V61" s="1"/>
       <c r="W61" s="1"/>
     </row>
-    <row r="62" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="N62" s="1"/>
@@ -13821,7 +13823,7 @@
       <c r="V62" s="1"/>
       <c r="W62" s="1"/>
     </row>
-    <row r="63" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="N63" s="1"/>
@@ -13832,7 +13834,7 @@
       <c r="V63" s="1"/>
       <c r="W63" s="1"/>
     </row>
-    <row r="64" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:39" x14ac:dyDescent="0.3">
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="N64" s="1"/>
@@ -13843,16 +13845,16 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
     </row>
-    <row r="66" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="10:23" x14ac:dyDescent="0.3">
       <c r="O66" s="1"/>
     </row>
-    <row r="69" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J69" s="1"/>
       <c r="N69" s="1"/>
       <c r="R69" s="1"/>
       <c r="V69" s="1"/>
     </row>
-    <row r="70" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="N70" s="1"/>
@@ -13863,7 +13865,7 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="71" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="71" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="N71" s="1"/>
@@ -13874,7 +13876,7 @@
       <c r="V71" s="1"/>
       <c r="W71" s="1"/>
     </row>
-    <row r="72" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="72" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="N72" s="1"/>
@@ -13885,7 +13887,7 @@
       <c r="V72" s="1"/>
       <c r="W72" s="1"/>
     </row>
-    <row r="73" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="73" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="N73" s="1"/>
@@ -13896,7 +13898,7 @@
       <c r="V73" s="1"/>
       <c r="W73" s="1"/>
     </row>
-    <row r="74" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="74" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="N74" s="1"/>
@@ -13907,7 +13909,7 @@
       <c r="V74" s="1"/>
       <c r="W74" s="1"/>
     </row>
-    <row r="75" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="N75" s="1"/>
@@ -13918,7 +13920,7 @@
       <c r="V75" s="1"/>
       <c r="W75" s="1"/>
     </row>
-    <row r="76" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="N76" s="1"/>
@@ -13929,13 +13931,13 @@
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
     </row>
-    <row r="81" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J81" s="1"/>
       <c r="N81" s="1"/>
       <c r="R81" s="1"/>
       <c r="V81" s="1"/>
     </row>
-    <row r="82" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="N82" s="1"/>
@@ -13946,7 +13948,7 @@
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
     </row>
-    <row r="83" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="83" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="N83" s="1"/>
@@ -13957,7 +13959,7 @@
       <c r="V83" s="1"/>
       <c r="W83" s="1"/>
     </row>
-    <row r="84" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="84" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="N84" s="1"/>
@@ -13968,7 +13970,7 @@
       <c r="V84" s="1"/>
       <c r="W84" s="1"/>
     </row>
-    <row r="85" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="85" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="N85" s="1"/>
@@ -13979,7 +13981,7 @@
       <c r="V85" s="1"/>
       <c r="W85" s="1"/>
     </row>
-    <row r="86" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="86" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="N86" s="1"/>
@@ -13990,7 +13992,7 @@
       <c r="V86" s="1"/>
       <c r="W86" s="1"/>
     </row>
-    <row r="87" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="N87" s="1"/>
@@ -14001,7 +14003,7 @@
       <c r="V87" s="1"/>
       <c r="W87" s="1"/>
     </row>
-    <row r="88" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="N88" s="1"/>
@@ -14012,13 +14014,13 @@
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
     </row>
-    <row r="93" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J93" s="1"/>
       <c r="N93" s="1"/>
       <c r="R93" s="1"/>
       <c r="V93" s="1"/>
     </row>
-    <row r="94" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="N94" s="1"/>
@@ -14029,7 +14031,7 @@
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
     </row>
-    <row r="95" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="95" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
       <c r="N95" s="1"/>
@@ -14040,7 +14042,7 @@
       <c r="V95" s="1"/>
       <c r="W95" s="1"/>
     </row>
-    <row r="96" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="96" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
       <c r="N96" s="1"/>
@@ -14051,7 +14053,7 @@
       <c r="V96" s="1"/>
       <c r="W96" s="1"/>
     </row>
-    <row r="97" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="97" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
       <c r="N97" s="1"/>
@@ -14062,7 +14064,7 @@
       <c r="V97" s="1"/>
       <c r="W97" s="1"/>
     </row>
-    <row r="98" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="98" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
       <c r="N98" s="1"/>
@@ -14073,7 +14075,7 @@
       <c r="V98" s="1"/>
       <c r="W98" s="1"/>
     </row>
-    <row r="99" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="N99" s="1"/>
@@ -14084,7 +14086,7 @@
       <c r="V99" s="1"/>
       <c r="W99" s="1"/>
     </row>
-    <row r="100" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="N100" s="1"/>
@@ -14095,13 +14097,13 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
     </row>
-    <row r="105" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J105" s="1"/>
       <c r="N105" s="1"/>
       <c r="R105" s="1"/>
       <c r="V105" s="1"/>
     </row>
-    <row r="106" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="N106" s="1"/>
@@ -14112,7 +14114,7 @@
       <c r="V106" s="1"/>
       <c r="W106" s="1"/>
     </row>
-    <row r="107" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="107" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="N107" s="1"/>
@@ -14123,7 +14125,7 @@
       <c r="V107" s="1"/>
       <c r="W107" s="1"/>
     </row>
-    <row r="108" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="108" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
       <c r="N108" s="1"/>
@@ -14134,7 +14136,7 @@
       <c r="V108" s="1"/>
       <c r="W108" s="1"/>
     </row>
-    <row r="109" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="109" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
       <c r="N109" s="1"/>
@@ -14145,7 +14147,7 @@
       <c r="V109" s="1"/>
       <c r="W109" s="1"/>
     </row>
-    <row r="110" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="110" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
       <c r="N110" s="1"/>
@@ -14156,7 +14158,7 @@
       <c r="V110" s="1"/>
       <c r="W110" s="1"/>
     </row>
-    <row r="111" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="111" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="N111" s="1"/>
@@ -14167,7 +14169,7 @@
       <c r="V111" s="1"/>
       <c r="W111" s="1"/>
     </row>
-    <row r="112" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="112" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="N112" s="1"/>
@@ -14178,13 +14180,13 @@
       <c r="V112" s="1"/>
       <c r="W112" s="1"/>
     </row>
-    <row r="117" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="117" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J117" s="1"/>
       <c r="N117" s="1"/>
       <c r="R117" s="1"/>
       <c r="V117" s="1"/>
     </row>
-    <row r="118" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="118" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
       <c r="N118" s="1"/>
@@ -14195,7 +14197,7 @@
       <c r="V118" s="1"/>
       <c r="W118" s="1"/>
     </row>
-    <row r="119" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="119" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
       <c r="N119" s="1"/>
@@ -14206,7 +14208,7 @@
       <c r="V119" s="1"/>
       <c r="W119" s="1"/>
     </row>
-    <row r="120" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="120" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="N120" s="1"/>
@@ -14217,7 +14219,7 @@
       <c r="V120" s="1"/>
       <c r="W120" s="1"/>
     </row>
-    <row r="121" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="121" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="N121" s="1"/>
@@ -14228,7 +14230,7 @@
       <c r="V121" s="1"/>
       <c r="W121" s="1"/>
     </row>
-    <row r="122" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="122" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="N122" s="1"/>
@@ -14239,7 +14241,7 @@
       <c r="V122" s="1"/>
       <c r="W122" s="1"/>
     </row>
-    <row r="123" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="123" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
       <c r="N123" s="1"/>
@@ -14250,7 +14252,7 @@
       <c r="V123" s="1"/>
       <c r="W123" s="1"/>
     </row>
-    <row r="124" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="124" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
       <c r="N124" s="1"/>
@@ -14284,33 +14286,33 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.109375" customWidth="1"/>
     <col min="2" max="2" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>53</v>
       </c>
@@ -14387,7 +14389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>135</v>
       </c>
@@ -14488,7 +14490,7 @@
         <v>0.4248242725493126</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -14514,7 +14516,7 @@
       <c r="X9" s="2"/>
       <c r="Y9" s="2"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -14543,109 +14545,109 @@
       <c r="X10" s="2"/>
       <c r="Y10" s="2"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>A7</f>
+        <f t="shared" ref="A11:Y11" si="4">A7</f>
         <v>Age</v>
       </c>
       <c r="B11" t="str">
-        <f>B7</f>
+        <f t="shared" si="4"/>
         <v>f.l.X0</v>
       </c>
       <c r="C11" t="str">
-        <f>C7</f>
+        <f t="shared" si="4"/>
         <v>f.l.X1</v>
       </c>
       <c r="D11" t="str">
-        <f>D7</f>
+        <f t="shared" si="4"/>
         <v>f.l.X2</v>
       </c>
       <c r="E11" t="str">
-        <f>E7</f>
+        <f t="shared" si="4"/>
         <v>f.l.X3</v>
       </c>
       <c r="F11" t="str">
-        <f>F7</f>
+        <f t="shared" si="4"/>
         <v>f.l.X4</v>
       </c>
       <c r="G11" t="str">
-        <f>G7</f>
+        <f t="shared" si="4"/>
         <v>f.l.X5</v>
       </c>
       <c r="H11" t="str">
-        <f>H7</f>
+        <f t="shared" si="4"/>
         <v>f.h.X0</v>
       </c>
       <c r="I11" t="str">
-        <f>I7</f>
+        <f t="shared" si="4"/>
         <v>f.h.X1</v>
       </c>
       <c r="J11" t="str">
-        <f>J7</f>
+        <f t="shared" si="4"/>
         <v>f.h.X2</v>
       </c>
       <c r="K11" t="str">
-        <f>K7</f>
+        <f t="shared" si="4"/>
         <v>f.h.X3</v>
       </c>
       <c r="L11" t="str">
-        <f>L7</f>
+        <f t="shared" si="4"/>
         <v>f.h.X4</v>
       </c>
       <c r="M11" t="str">
-        <f>M7</f>
+        <f t="shared" si="4"/>
         <v>f.h.X5</v>
       </c>
       <c r="N11" t="str">
-        <f>N7</f>
+        <f t="shared" si="4"/>
         <v>m.l.X0</v>
       </c>
       <c r="O11" t="str">
-        <f>O7</f>
+        <f t="shared" si="4"/>
         <v>m.l.X1</v>
       </c>
       <c r="P11" t="str">
-        <f>P7</f>
+        <f t="shared" si="4"/>
         <v>m.l.X2</v>
       </c>
       <c r="Q11" t="str">
-        <f>Q7</f>
+        <f t="shared" si="4"/>
         <v>m.l.X3</v>
       </c>
       <c r="R11" t="str">
-        <f>R7</f>
+        <f t="shared" si="4"/>
         <v>m.l.X4</v>
       </c>
       <c r="S11" t="str">
-        <f>S7</f>
+        <f t="shared" si="4"/>
         <v>m.l.X5</v>
       </c>
       <c r="T11" t="str">
-        <f>T7</f>
+        <f t="shared" si="4"/>
         <v>m.h.X0</v>
       </c>
       <c r="U11" t="str">
-        <f>U7</f>
+        <f t="shared" si="4"/>
         <v>m.h.X1</v>
       </c>
       <c r="V11" t="str">
-        <f>V7</f>
+        <f t="shared" si="4"/>
         <v>m.h.X2</v>
       </c>
       <c r="W11" t="str">
-        <f>W7</f>
+        <f t="shared" si="4"/>
         <v>m.h.X3</v>
       </c>
       <c r="X11" t="str">
-        <f>X7</f>
+        <f t="shared" si="4"/>
         <v>m.h.X4</v>
       </c>
       <c r="Y11" t="str">
-        <f>Y7</f>
+        <f t="shared" si="4"/>
         <v>m.h.X5</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>135</v>
       </c>
@@ -14658,19 +14660,19 @@
         <v>0.34029048249791771</v>
       </c>
       <c r="D12" s="2">
-        <f t="shared" ref="D12:G12" si="4">C12</f>
+        <f t="shared" ref="D12:G12" si="5">C12</f>
         <v>0.34029048249791771</v>
       </c>
       <c r="E12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34029048249791771</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34029048249791771</v>
       </c>
       <c r="G12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.34029048249791771</v>
       </c>
       <c r="H12" s="2">
@@ -14682,19 +14684,19 @@
         <v>0.27249512024599126</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" ref="J12:M12" si="5">I12</f>
+        <f t="shared" ref="J12:M12" si="6">I12</f>
         <v>0.27249512024599126</v>
       </c>
       <c r="K12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27249512024599126</v>
       </c>
       <c r="L12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27249512024599126</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.27249512024599126</v>
       </c>
       <c r="N12" s="2">
@@ -14706,19 +14708,19 @@
         <v>0.37613168601042085</v>
       </c>
       <c r="P12" s="2">
-        <f t="shared" ref="P12:S12" si="6">O12</f>
+        <f t="shared" ref="P12:S12" si="7">O12</f>
         <v>0.37613168601042085</v>
       </c>
       <c r="Q12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.37613168601042085</v>
       </c>
       <c r="R12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.37613168601042085</v>
       </c>
       <c r="S12" s="2">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.37613168601042085</v>
       </c>
       <c r="T12" s="2">
@@ -14730,28 +14732,28 @@
         <v>0.30449151282646025</v>
       </c>
       <c r="V12" s="2">
-        <f t="shared" ref="V12:Y12" si="7">U12</f>
+        <f t="shared" ref="V12:Y12" si="8">U12</f>
         <v>0.30449151282646025</v>
       </c>
       <c r="W12" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.30449151282646025</v>
       </c>
       <c r="X12" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.30449151282646025</v>
       </c>
       <c r="Y12" s="2">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.30449151282646025</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>58</v>
       </c>
@@ -14776,7 +14778,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A22" s="39"/>
       <c r="B22" s="40"/>
       <c r="C22" s="43" t="s">
@@ -14820,7 +14822,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="41"/>
       <c r="B23" s="42"/>
       <c r="C23" s="44"/>
@@ -14840,7 +14842,7 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
         <v>133</v>
       </c>
@@ -14890,7 +14892,7 @@
       </c>
       <c r="S24" s="7"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="23"/>
       <c r="B25" s="12" t="s">
         <v>41</v>
@@ -14938,7 +14940,7 @@
       </c>
       <c r="S25" s="7"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="12" t="s">
         <v>42</v>
@@ -14967,11 +14969,11 @@
         <v>18</v>
       </c>
       <c r="L26" s="7">
-        <f t="shared" ref="L26:M26" si="8">K26</f>
+        <f t="shared" ref="L26:M26" si="9">K26</f>
         <v>18</v>
       </c>
       <c r="M26" s="7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="N26" s="7"/>
@@ -14979,20 +14981,20 @@
         <v>18</v>
       </c>
       <c r="P26" s="7">
-        <f t="shared" ref="P26:R26" si="9">O26</f>
+        <f t="shared" ref="P26:R26" si="10">O26</f>
         <v>18</v>
       </c>
       <c r="Q26" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="R26" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="S26" s="7"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="12" t="s">
         <v>43</v>
@@ -15040,7 +15042,7 @@
       </c>
       <c r="S27" s="7"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="12" t="s">
         <v>44</v>
@@ -15088,7 +15090,7 @@
       </c>
       <c r="S28" s="7"/>
     </row>
-    <row r="29" spans="1:19" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="12" t="s">
         <v>56</v>
@@ -15136,7 +15138,7 @@
       </c>
       <c r="S29" s="7"/>
     </row>
-    <row r="30" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="18"/>
       <c r="B30" s="19" t="s">
         <v>45</v>
@@ -15184,56 +15186,56 @@
       </c>
       <c r="S30" s="7"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
       <c r="H31" s="3"/>
       <c r="J31">
         <f>J24*$C24+J25*$C25+J26*$C26+J27*$C27+J28*$C28+J29*$C29+J30*$C30</f>
         <v>1.699999999999996E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" ref="K31:R31" si="10">K24*$C24+K25*$C25+K26*$C26+K27*$C27+K28*$C28+K29*$C29+K30*$C30</f>
+        <f t="shared" ref="K31:R31" si="11">K24*$C24+K25*$C25+K26*$C26+K27*$C27+K28*$C28+K29*$C29+K30*$C30</f>
         <v>-0.13900000000000001</v>
       </c>
       <c r="L31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.30300000000000005</v>
       </c>
       <c r="M31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.45900000000000002</v>
       </c>
       <c r="O31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.50600000000000001</v>
       </c>
       <c r="P31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.66200000000000014</v>
       </c>
       <c r="Q31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.82600000000000007</v>
       </c>
       <c r="R31">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-0.98199999999999998</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
       <c r="J32">
         <f>EXP(-J31)</f>
         <v>0.98314368463490964</v>
       </c>
       <c r="K32">
-        <f t="shared" ref="K32:M32" si="11">EXP(-K31)</f>
+        <f t="shared" ref="K32:M32" si="12">EXP(-K31)</f>
         <v>1.1491241000036052</v>
       </c>
       <c r="L32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.3539144644422885</v>
       </c>
       <c r="M32">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1.5824907027825335</v>
       </c>
       <c r="O32">
@@ -15253,7 +15255,7 @@
         <v>2.669790486880145</v>
       </c>
     </row>
-    <row r="33" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:32" x14ac:dyDescent="0.3">
       <c r="I33" t="s">
         <v>46</v>
       </c>
@@ -15262,44 +15264,44 @@
         <v>0.50424989764879125</v>
       </c>
       <c r="K33" s="1">
-        <f t="shared" ref="K33:M33" si="12">1/(1+K32)</f>
+        <f t="shared" ref="K33:M33" si="13">1/(1+K32)</f>
         <v>0.46530584250501056</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.4248242725493126</v>
       </c>
       <c r="M33" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.3872230784500168</v>
       </c>
       <c r="N33" s="1"/>
       <c r="O33" s="1">
-        <f t="shared" ref="O33:R33" si="13">1/(1+O32)</f>
+        <f t="shared" ref="O33:R33" si="14">1/(1+O32)</f>
         <v>0.37613168601042085</v>
       </c>
       <c r="P33" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.34029048249791771</v>
       </c>
       <c r="Q33" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30449151282646025</v>
       </c>
       <c r="R33" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.27249512024599126</v>
       </c>
       <c r="S33" s="1"/>
     </row>
-    <row r="34" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O34" s="1"/>
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
     </row>
-    <row r="35" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
@@ -15312,7 +15314,7 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="1"/>
     </row>
-    <row r="36" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C36" s="11"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
@@ -15326,17 +15328,17 @@
       <c r="X36" s="1"/>
       <c r="Y36" s="1"/>
     </row>
-    <row r="38" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
     </row>
-    <row r="39" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="J39" s="1"/>
       <c r="N39" s="1"/>
       <c r="R39" s="1"/>
       <c r="V39" s="1"/>
     </row>
-    <row r="40" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -15348,7 +15350,7 @@
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
     </row>
-    <row r="41" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="N41" s="1"/>
@@ -15360,7 +15362,7 @@
       <c r="W41" s="1"/>
       <c r="Z41" s="1"/>
     </row>
-    <row r="42" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="N42" s="1"/>
@@ -15372,7 +15374,7 @@
       <c r="W42" s="1"/>
       <c r="Z42" s="1"/>
     </row>
-    <row r="43" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="N43" s="1"/>
@@ -15383,7 +15385,7 @@
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
     </row>
-    <row r="44" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="N44" s="1"/>
@@ -15394,7 +15396,7 @@
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
     </row>
-    <row r="45" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="N45" s="1"/>
@@ -15405,7 +15407,7 @@
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
     </row>
-    <row r="46" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:32" x14ac:dyDescent="0.3">
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="N46" s="1"/>
@@ -15416,10 +15418,10 @@
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
     </row>
-    <row r="47" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:32" x14ac:dyDescent="0.3">
       <c r="AA47" s="1"/>
     </row>
-    <row r="48" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:32" x14ac:dyDescent="0.3">
       <c r="O48" s="1"/>
       <c r="AA48" s="1"/>
       <c r="AB48" s="1"/>
@@ -15428,13 +15430,13 @@
       <c r="AE48" s="1"/>
       <c r="AF48" s="1"/>
     </row>
-    <row r="51" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="51" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J51" s="1"/>
       <c r="N51" s="1"/>
       <c r="R51" s="1"/>
       <c r="V51" s="1"/>
     </row>
-    <row r="52" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="52" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="N52" s="1"/>
@@ -15445,7 +15447,7 @@
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
     </row>
-    <row r="53" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="53" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="N53" s="1"/>
@@ -15456,7 +15458,7 @@
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
     </row>
-    <row r="54" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="54" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="N54" s="1"/>
@@ -15467,7 +15469,7 @@
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
     </row>
-    <row r="55" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="55" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="N55" s="1"/>
@@ -15478,7 +15480,7 @@
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
     </row>
-    <row r="56" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="56" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="N56" s="1"/>
@@ -15489,7 +15491,7 @@
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
     </row>
-    <row r="57" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="57" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="N57" s="1"/>
@@ -15500,7 +15502,7 @@
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
     </row>
-    <row r="58" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="58" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="N58" s="1"/>
@@ -15511,13 +15513,13 @@
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
     </row>
-    <row r="63" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J63" s="1"/>
       <c r="N63" s="1"/>
       <c r="R63" s="1"/>
       <c r="V63" s="1"/>
     </row>
-    <row r="64" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="N64" s="1"/>
@@ -15528,7 +15530,7 @@
       <c r="V64" s="1"/>
       <c r="W64" s="1"/>
     </row>
-    <row r="65" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="65" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="N65" s="1"/>
@@ -15539,7 +15541,7 @@
       <c r="V65" s="1"/>
       <c r="W65" s="1"/>
     </row>
-    <row r="66" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="66" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="N66" s="1"/>
@@ -15550,7 +15552,7 @@
       <c r="V66" s="1"/>
       <c r="W66" s="1"/>
     </row>
-    <row r="67" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="67" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="N67" s="1"/>
@@ -15561,7 +15563,7 @@
       <c r="V67" s="1"/>
       <c r="W67" s="1"/>
     </row>
-    <row r="68" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="68" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="N68" s="1"/>
@@ -15572,7 +15574,7 @@
       <c r="V68" s="1"/>
       <c r="W68" s="1"/>
     </row>
-    <row r="69" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="69" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="N69" s="1"/>
@@ -15583,7 +15585,7 @@
       <c r="V69" s="1"/>
       <c r="W69" s="1"/>
     </row>
-    <row r="70" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="70" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="N70" s="1"/>
@@ -15594,13 +15596,13 @@
       <c r="V70" s="1"/>
       <c r="W70" s="1"/>
     </row>
-    <row r="75" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="75" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J75" s="1"/>
       <c r="N75" s="1"/>
       <c r="R75" s="1"/>
       <c r="V75" s="1"/>
     </row>
-    <row r="76" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="76" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="N76" s="1"/>
@@ -15611,7 +15613,7 @@
       <c r="V76" s="1"/>
       <c r="W76" s="1"/>
     </row>
-    <row r="77" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="77" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="N77" s="1"/>
@@ -15622,7 +15624,7 @@
       <c r="V77" s="1"/>
       <c r="W77" s="1"/>
     </row>
-    <row r="78" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="78" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="N78" s="1"/>
@@ -15633,7 +15635,7 @@
       <c r="V78" s="1"/>
       <c r="W78" s="1"/>
     </row>
-    <row r="79" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="79" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="N79" s="1"/>
@@ -15644,7 +15646,7 @@
       <c r="V79" s="1"/>
       <c r="W79" s="1"/>
     </row>
-    <row r="80" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="80" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="N80" s="1"/>
@@ -15655,7 +15657,7 @@
       <c r="V80" s="1"/>
       <c r="W80" s="1"/>
     </row>
-    <row r="81" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="81" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="N81" s="1"/>
@@ -15666,7 +15668,7 @@
       <c r="V81" s="1"/>
       <c r="W81" s="1"/>
     </row>
-    <row r="82" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="82" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="N82" s="1"/>
@@ -15677,13 +15679,13 @@
       <c r="V82" s="1"/>
       <c r="W82" s="1"/>
     </row>
-    <row r="87" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="87" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J87" s="1"/>
       <c r="N87" s="1"/>
       <c r="R87" s="1"/>
       <c r="V87" s="1"/>
     </row>
-    <row r="88" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="88" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="N88" s="1"/>
@@ -15694,7 +15696,7 @@
       <c r="V88" s="1"/>
       <c r="W88" s="1"/>
     </row>
-    <row r="89" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="89" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="N89" s="1"/>
@@ -15705,7 +15707,7 @@
       <c r="V89" s="1"/>
       <c r="W89" s="1"/>
     </row>
-    <row r="90" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="90" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
       <c r="N90" s="1"/>
@@ -15716,7 +15718,7 @@
       <c r="V90" s="1"/>
       <c r="W90" s="1"/>
     </row>
-    <row r="91" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="91" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="N91" s="1"/>
@@ -15727,7 +15729,7 @@
       <c r="V91" s="1"/>
       <c r="W91" s="1"/>
     </row>
-    <row r="92" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="92" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="N92" s="1"/>
@@ -15738,7 +15740,7 @@
       <c r="V92" s="1"/>
       <c r="W92" s="1"/>
     </row>
-    <row r="93" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="93" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="N93" s="1"/>
@@ -15749,7 +15751,7 @@
       <c r="V93" s="1"/>
       <c r="W93" s="1"/>
     </row>
-    <row r="94" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="94" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="N94" s="1"/>
@@ -15760,13 +15762,13 @@
       <c r="V94" s="1"/>
       <c r="W94" s="1"/>
     </row>
-    <row r="99" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="99" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J99" s="1"/>
       <c r="N99" s="1"/>
       <c r="R99" s="1"/>
       <c r="V99" s="1"/>
     </row>
-    <row r="100" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="100" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="N100" s="1"/>
@@ -15777,7 +15779,7 @@
       <c r="V100" s="1"/>
       <c r="W100" s="1"/>
     </row>
-    <row r="101" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="101" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="N101" s="1"/>
@@ -15788,7 +15790,7 @@
       <c r="V101" s="1"/>
       <c r="W101" s="1"/>
     </row>
-    <row r="102" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="102" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="N102" s="1"/>
@@ -15799,7 +15801,7 @@
       <c r="V102" s="1"/>
       <c r="W102" s="1"/>
     </row>
-    <row r="103" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="103" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="N103" s="1"/>
@@ -15810,7 +15812,7 @@
       <c r="V103" s="1"/>
       <c r="W103" s="1"/>
     </row>
-    <row r="104" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="104" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="N104" s="1"/>
@@ -15821,7 +15823,7 @@
       <c r="V104" s="1"/>
       <c r="W104" s="1"/>
     </row>
-    <row r="105" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="105" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="N105" s="1"/>
@@ -15832,7 +15834,7 @@
       <c r="V105" s="1"/>
       <c r="W105" s="1"/>
     </row>
-    <row r="106" spans="10:23" x14ac:dyDescent="0.25">
+    <row r="106" spans="10:23" x14ac:dyDescent="0.3">
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="N106" s="1"/>
@@ -15845,12 +15847,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="G22:G23"/>
     <mergeCell ref="A22:B23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>